<commit_message>
All tests running now but 1.5!
Split up into seperate tests to make finding errors/assertion failures
easier; currently having trouble with 'exiting' the room the same way
you came in
</commit_message>
<xml_diff>
--- a/ClueLayout_With_Tests.xlsx
+++ b/ClueLayout_With_Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="580" windowWidth="15860" windowHeight="14120"/>
+    <workbookView xWindow="14760" yWindow="600" windowWidth="14460" windowHeight="14260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="75">
   <si>
     <t>Turqoise: Targets calculated when leaving a room</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -774,7 +774,7 @@
   <dimension ref="A1:Y36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -831,8 +831,8 @@
       <c r="P1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="26" t="s">
-        <v>29</v>
+      <c r="Q1" s="26">
+        <v>1</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>29</v>
@@ -1059,8 +1059,8 @@
       <c r="O4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="27" t="s">
-        <v>29</v>
+      <c r="P4" s="27">
+        <v>1</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>29</v>
@@ -1453,14 +1453,14 @@
       <c r="R9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="S9" s="27" t="s">
-        <v>29</v>
+      <c r="S9" s="27">
+        <v>2</v>
       </c>
       <c r="T9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="U9" s="26" t="s">
-        <v>29</v>
+      <c r="U9" s="26">
+        <v>3</v>
       </c>
       <c r="V9" s="3" t="s">
         <v>29</v>
@@ -1574,8 +1574,8 @@
       <c r="G11" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="H11" s="26" t="s">
-        <v>29</v>
+      <c r="H11" s="26">
+        <v>2</v>
       </c>
       <c r="I11" s="19" t="s">
         <v>54</v>
@@ -2069,8 +2069,8 @@
       <c r="R17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="S17" s="28" t="s">
-        <v>29</v>
+      <c r="S17" s="28">
+        <v>1</v>
       </c>
       <c r="T17" s="3" t="s">
         <v>29</v>
@@ -2081,8 +2081,8 @@
       <c r="V17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="W17" s="28" t="s">
-        <v>29</v>
+      <c r="W17" s="28">
+        <v>1</v>
       </c>
       <c r="X17" s="3" t="s">
         <v>29</v>
@@ -2193,8 +2193,8 @@
       <c r="H19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="26" t="s">
-        <v>29</v>
+      <c r="I19" s="26">
+        <v>4</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>7</v>
@@ -2365,14 +2365,14 @@
       <c r="N21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O21" s="28" t="s">
-        <v>29</v>
+      <c r="O21" s="28">
+        <v>2</v>
       </c>
       <c r="P21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q21" s="28" t="s">
-        <v>29</v>
+      <c r="Q21" s="28">
+        <v>2</v>
       </c>
       <c r="R21" s="2" t="s">
         <v>10</v>
@@ -2445,8 +2445,8 @@
       <c r="O22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P22" s="28" t="s">
-        <v>29</v>
+      <c r="P22" s="28">
+        <v>2</v>
       </c>
       <c r="Q22" s="3" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Made fix for entering room- all tests passing
Added an if-statement inside of calcTargets
</commit_message>
<xml_diff>
--- a/ClueLayout_With_Tests.xlsx
+++ b/ClueLayout_With_Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="2540" windowWidth="24800" windowHeight="16100"/>
+    <workbookView xWindow="15820" yWindow="2360" windowWidth="24800" windowHeight="16100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -778,7 +778,7 @@
   <dimension ref="A1:Y36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -2863,6 +2863,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2881,6 +2882,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -2898,6 +2900,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>